<commit_message>
Updated Reports & scenario col added in td
</commit_message>
<xml_diff>
--- a/testdata/testdata-API.xlsx
+++ b/testdata/testdata-API.xlsx
@@ -21,11 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t xml:space="preserve">Execute?</t>
   </si>
   <si>
+    <t xml:space="preserve">Scenario</t>
+  </si>
+  <si>
     <t xml:space="preserve">URI</t>
   </si>
   <si>
@@ -41,22 +44,28 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
+    <t xml:space="preserve">Valid</t>
+  </si>
+  <si>
     <t xml:space="preserve">/users/zpaya</t>
   </si>
   <si>
     <t xml:space="preserve">zpaya</t>
   </si>
   <si>
+    <t xml:space="preserve">Invalid URI</t>
+  </si>
+  <si>
     <t xml:space="preserve">/users/zpaya1</t>
   </si>
   <si>
     <t xml:space="preserve">na</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
     <t xml:space="preserve">/users/zpayaInvalid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -180,12 +189,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,27 +231,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.62753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.03238866396761"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -250,90 +264,68 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="n">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>3122759</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="n">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="n">
         <v>204</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>404</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>3122759</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>3122759</v>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -361,132 +353,132 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>6160393</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>404</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>6160393</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>404</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>6160393</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>11471217</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="n">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>55369183</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>77030017</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>